<commit_message>
Excel sample image added for helping examiner using modal view
</commit_message>
<xml_diff>
--- a/ExamPortal/backend/backend_nodejs/upload/updated.xlsx
+++ b/ExamPortal/backend/backend_nodejs/upload/updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashish.chopra\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{29D6D9EB-F4EB-4FEE-8AC6-6B9FFAB154FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{202D209F-4B60-4D13-BD6C-97ABC681D04B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{C5F203CF-F3BD-4073-B241-D27D6AA751EF}"/>
   </bookViews>
@@ -28,87 +28,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="32" uniqueCount="27">
-  <si>
-    <t>Bhutan</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Pakistan</t>
-  </si>
-  <si>
-    <t>Where is Birendra from?</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>Bhjutan</t>
-  </si>
-  <si>
-    <t>usa</t>
-  </si>
-  <si>
-    <t>mexico</t>
-  </si>
-  <si>
-    <t>elchapo</t>
-  </si>
-  <si>
-    <t>Where is Ashish From?</t>
-  </si>
-  <si>
-    <t>Saharanpur</t>
-  </si>
-  <si>
-    <t>Noida</t>
-  </si>
-  <si>
-    <t>Mumbai</t>
-  </si>
-  <si>
-    <t>Las Vegas</t>
-  </si>
-  <si>
-    <t>url('www.usa.com')</t>
-  </si>
-  <si>
-    <t>option1</t>
-  </si>
-  <si>
-    <t>option4</t>
-  </si>
-  <si>
-    <t>computer was invented by?</t>
-  </si>
-  <si>
-    <t>chopra</t>
-  </si>
-  <si>
-    <t>rawat</t>
-  </si>
-  <si>
-    <t>birendra</t>
-  </si>
-  <si>
-    <t>chandan</t>
-  </si>
-  <si>
-    <t>www.chopra.com</t>
-  </si>
-  <si>
-    <t>multipleOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> option1 option2 option3</t>
-  </si>
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="8" uniqueCount="8">
   <si>
     <t>singleOption</t>
+  </si>
+  <si>
+    <t>who is the richest man in the world?</t>
+  </si>
+  <si>
+    <t>Mukesh Ambani</t>
+  </si>
+  <si>
+    <t>Bill Gates</t>
+  </si>
+  <si>
+    <t>Jeff Bezos</t>
+  </si>
+  <si>
+    <t>Warren Buffet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> option3</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -474,138 +417,54 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E608057-4077-4E87-A5E5-F07480B12DDB}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.85546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" customWidth="1"/>
     <col min="9" max="9" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="G1">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
+      <c r="H4" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{DA4252DC-5F0E-4FE9-A51C-561C0C5CC64A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>